<commit_message>
system test case v1
</commit_message>
<xml_diff>
--- a/DesignDocument/(5Team_Test_003) Test case.xlsx
+++ b/DesignDocument/(5Team_Test_003) Test case.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanghee3.lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\surepark\SureParkSystem\DesignDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="45" windowWidth="15075" windowHeight="10485" activeTab="2"/>
+    <workbookView xWindow="2400" yWindow="45" windowWidth="15075" windowHeight="10485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="(Integration) 1. Manage" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="308">
   <si>
     <t>TC ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1065,11 +1065,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. SE-2(ParkingLot) is connected to SE-01(ParkServer).
-2. Driver arrived at entry gate.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">1. SE-6(ParkView) display "welcome message" when receive a message from SE-1(ParkServer)
  </t>
@@ -1251,7 +1246,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>※ 통계정보 표시를 위한 준비사항 확인.</t>
+    <t>Procedure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Driver arrived at entry gate.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. owner로 log-in 한다.
+2. server에 1년치 데이터를 보유하고 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Owner가 parking lot 을 선택한다.
+2. 통계 기간을 선택한다.
+3. 통계 정보를 요청한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 해당 parking lot의 현재 주차 상태를 보인다.
+2. 해당 기간의 점유율, 매출, 취소율이 표시된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. attendant로 log-in 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1381,7 +1408,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1494,6 +1521,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1801,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K4"/>
+  <dimension ref="B2:L7"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1821,7 +1851,7 @@
     <col min="12" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="27" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="229.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="229.5" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>257</v>
       </c>
@@ -1867,10 +1897,10 @@
         <v>219</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1879,7 +1909,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="229.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="229.5" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>259</v>
       </c>
@@ -1893,10 +1923,10 @@
         <v>221</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1904,6 +1934,69 @@
       <c r="K4" s="29" t="s">
         <v>244</v>
       </c>
+    </row>
+    <row r="5" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="30"/>
+    </row>
+    <row r="6" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="30"/>
+    </row>
+    <row r="7" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>233</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1980,10 +2073,10 @@
         <v>155</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H3" s="33"/>
       <c r="I3" s="4"/>
@@ -2006,16 +2099,16 @@
         <v>160</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="162" x14ac:dyDescent="0.3">
@@ -2032,10 +2125,10 @@
         <v>161</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -2058,10 +2151,10 @@
         <v>162</v>
       </c>
       <c r="F6" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>287</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2082,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K28"/>
+  <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2094,13 +2187,14 @@
     <col min="4" max="4" width="9" style="9"/>
     <col min="5" max="5" width="50.125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.25" customWidth="1"/>
-    <col min="7" max="7" width="86.625" customWidth="1"/>
-    <col min="8" max="8" width="18.125" customWidth="1"/>
-    <col min="10" max="10" width="15.875" customWidth="1"/>
-    <col min="11" max="11" width="42.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.25" style="20" customWidth="1"/>
+    <col min="8" max="8" width="86.625" customWidth="1"/>
+    <col min="9" max="9" width="18.125" customWidth="1"/>
+    <col min="11" max="11" width="15.875" customWidth="1"/>
+    <col min="12" max="12" width="42.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="27" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>84</v>
       </c>
@@ -2117,22 +2211,25 @@
         <v>87</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="94.5" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>34</v>
       </c>
@@ -2146,23 +2243,26 @@
         <v>115</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>280</v>
+        <v>121</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="8"/>
+      <c r="L3" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>35</v>
       </c>
@@ -2178,17 +2278,18 @@
       <c r="F4" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>280</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="54" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -2204,17 +2305,18 @@
       <c r="F5" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>40</v>
       </c>
@@ -2230,17 +2332,18 @@
       <c r="F6" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2256,17 +2359,18 @@
       <c r="F7" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
@@ -2282,17 +2386,18 @@
       <c r="F8" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
@@ -2308,17 +2413,18 @@
       <c r="F9" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
@@ -2334,17 +2440,18 @@
       <c r="F10" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -2360,15 +2467,16 @@
       <c r="F11" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="2:11" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="K11" s="4"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -2384,17 +2492,18 @@
       <c r="F12" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -2410,17 +2519,18 @@
       <c r="F13" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="4"/>
+      <c r="L13" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="94.5" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>53</v>
       </c>
@@ -2436,17 +2546,18 @@
       <c r="F14" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
@@ -2462,17 +2573,18 @@
       <c r="F15" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="4"/>
+      <c r="L15" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>55</v>
       </c>
@@ -2488,17 +2600,18 @@
       <c r="F16" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>58</v>
       </c>
@@ -2514,17 +2627,18 @@
       <c r="F17" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="4"/>
+      <c r="L17" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="67.5" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>59</v>
       </c>
@@ -2540,45 +2654,46 @@
       <c r="F18" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G21" s="20"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="20"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2589,10 +2704,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K44"/>
+  <dimension ref="B2:L41"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2600,16 +2715,16 @@
     <col min="1" max="1" width="3" style="20" customWidth="1"/>
     <col min="2" max="4" width="9" style="20"/>
     <col min="5" max="5" width="73.125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="27.25" style="20" customWidth="1"/>
-    <col min="8" max="8" width="19.375" style="20" customWidth="1"/>
-    <col min="9" max="9" width="9" style="20"/>
-    <col min="10" max="10" width="15.875" style="20" customWidth="1"/>
-    <col min="11" max="11" width="42.25" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="20"/>
+    <col min="6" max="7" width="38.875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="39.375" style="20" customWidth="1"/>
+    <col min="9" max="9" width="19.375" style="20" customWidth="1"/>
+    <col min="10" max="10" width="9" style="20"/>
+    <col min="11" max="11" width="15.875" style="20" customWidth="1"/>
+    <col min="12" max="12" width="42.25" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="27" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2626,24 +2741,27 @@
         <v>33</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="324" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>186</v>
@@ -2654,20 +2772,23 @@
       <c r="E3" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="H3" s="4"/>
+      <c r="F3" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>303</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>304</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="28" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>253</v>
       </c>
@@ -2681,17 +2802,22 @@
         <v>215</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+        <v>305</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>254</v>
       </c>
@@ -2704,16 +2830,23 @@
       <c r="E5" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B6" s="34" t="s">
         <v>255</v>
       </c>
@@ -2726,16 +2859,23 @@
       <c r="E6" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>306</v>
+      </c>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="35"/>
+      <c r="L6" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" s="36" customFormat="1" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B7" s="34" t="s">
         <v>256</v>
       </c>
@@ -2748,16 +2888,23 @@
       <c r="E7" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="F7" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>306</v>
+      </c>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="35"/>
+      <c r="L7" s="28" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="38.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="38.25" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>258</v>
       </c>
@@ -2770,14 +2917,17 @@
       <c r="E8" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="G8" s="18"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="27"/>
-    </row>
-    <row r="9" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K8" s="4"/>
+      <c r="L8" s="27"/>
+    </row>
+    <row r="9" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>260</v>
       </c>
@@ -2791,15 +2941,16 @@
         <v>222</v>
       </c>
       <c r="F9" s="18"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="29" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>261</v>
       </c>
@@ -2813,15 +2964,16 @@
         <v>223</v>
       </c>
       <c r="F10" s="18"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="29" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>262</v>
       </c>
@@ -2835,15 +2987,16 @@
         <v>224</v>
       </c>
       <c r="F11" s="18"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="31" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="31" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>263</v>
       </c>
@@ -2857,13 +3010,14 @@
         <v>225</v>
       </c>
       <c r="F12" s="18"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="30"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="4"/>
+      <c r="L12" s="30"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>264</v>
       </c>
@@ -2877,13 +3031,14 @@
         <v>226</v>
       </c>
       <c r="F13" s="18"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="29"/>
-    </row>
-    <row r="14" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K13" s="4"/>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>265</v>
       </c>
@@ -2897,13 +3052,14 @@
         <v>227</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="30"/>
-    </row>
-    <row r="15" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K14" s="1"/>
+      <c r="L14" s="30"/>
+    </row>
+    <row r="15" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>266</v>
       </c>
@@ -2917,15 +3073,16 @@
         <v>228</v>
       </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="1"/>
+      <c r="L15" s="31" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>267</v>
       </c>
@@ -2939,13 +3096,14 @@
         <v>229</v>
       </c>
       <c r="F16" s="18"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="30"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K16" s="1"/>
+      <c r="L16" s="30"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>268</v>
       </c>
@@ -2959,593 +3117,558 @@
         <v>230</v>
       </c>
       <c r="F17" s="18"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="30"/>
-    </row>
-    <row r="18" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K17" s="1"/>
+      <c r="L17" s="30"/>
+    </row>
+    <row r="18" spans="2:12" ht="51" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>231</v>
+        <v>112</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>234</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="30"/>
-    </row>
-    <row r="19" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K18" s="1"/>
+      <c r="L18" s="31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="54" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="8" t="s">
+        <v>289</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="30"/>
-    </row>
-    <row r="20" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K19" s="1"/>
+      <c r="L19" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>150</v>
+        <v>211</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="30"/>
-    </row>
-    <row r="21" spans="2:11" ht="51" x14ac:dyDescent="0.3">
+      <c r="K20" s="1"/>
+      <c r="L20" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="54" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>112</v>
+        <v>211</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="8" t="s">
+        <v>290</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="31" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="K21" s="1"/>
+      <c r="L21" s="31" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>211</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="H22" s="1"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="37" t="s">
+        <v>291</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="30" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K22" s="1"/>
+      <c r="L22" s="31" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>274</v>
+        <v>185</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="30" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="I23" s="33"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>275</v>
+        <v>172</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="31" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>276</v>
+        <v>173</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F26" s="18"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="33"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K26" s="4"/>
+      <c r="L26" s="28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F27" s="18"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K27" s="4"/>
+      <c r="L27" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>153</v>
+        <v>281</v>
       </c>
       <c r="F28" s="18"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="29"/>
-    </row>
-    <row r="29" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K28" s="4"/>
+      <c r="L28" s="28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F29" s="18"/>
-      <c r="G29" s="4"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K29" s="4"/>
+      <c r="L29" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F30" s="18"/>
-      <c r="G30" s="4"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K30" s="4"/>
+      <c r="L30" s="29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>282</v>
+        <v>159</v>
       </c>
       <c r="F31" s="18"/>
-      <c r="G31" s="4"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="28" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K31" s="4"/>
+      <c r="L31" s="29"/>
+    </row>
+    <row r="32" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="F32" s="18"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="28" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K32" s="4"/>
+      <c r="L32" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
-        <v>179</v>
+        <v>38</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="F33" s="18"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="29" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K33" s="4"/>
+      <c r="L33" s="27"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>114</v>
+        <v>7</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>159</v>
+        <v>63</v>
       </c>
       <c r="F34" s="18"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="29"/>
-    </row>
-    <row r="35" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K34" s="4"/>
+      <c r="L34" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>111</v>
+        <v>12</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K35" s="4"/>
+      <c r="L35" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>112</v>
+        <v>17</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>110</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="27"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K36" s="4"/>
+      <c r="L36" s="27"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>112</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F37" s="18"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
-      <c r="K37" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K37" s="4"/>
+      <c r="L37" s="27"/>
+    </row>
+    <row r="38" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="18"/>
-      <c r="G38" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K38" s="4"/>
+      <c r="L38" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>110</v>
+        <v>20</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>112</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F39" s="18"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="27"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K39" s="4"/>
+      <c r="L39" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>112</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F40" s="18"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
-      <c r="K40" s="27"/>
-    </row>
-    <row r="41" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="K40" s="4"/>
+      <c r="L40" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="19"/>
-      <c r="G41" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="18"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="B43" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F43" s="18"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" ht="25.5" x14ac:dyDescent="0.3">
-      <c r="B44" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44" s="18"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="28" t="s">
+      <c r="K41" s="4"/>
+      <c r="L41" s="28" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>